<commit_message>
ADD new lab files and other data
</commit_message>
<xml_diff>
--- a/sem2/MCH/lab1.01/Data.xlsx
+++ b/sem2/MCH/lab1.01/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilyaa/iDevelop/itmo-uni/sem2/MCH/lab1.01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3359090C-D1A6-C446-A194-885805270A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B4D253-9B3A-0C44-A635-BC9721E4C71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{42337130-DB75-304D-8F6A-7B155FC8FB3B}"/>
   </bookViews>
@@ -16,32 +16,39 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Лист1!$O$28:$O$37</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Лист1!$P$28:$P$37</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Лист1!$O$28:$O$37</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Лист1!$P$28:$P$37</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Лист1!$O$28:$O$37</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Лист1!$P$28:$P$37</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Лист1!$O$28:$O$37</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Лист1!$P$28:$P$37</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Лист1!$O$28:$O$37</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Лист1!$P$28:$P$37</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Лист1!$O$28:$O$37</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Лист1!$P$28:$P$37</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Лист1!$O$28:$O$37</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Лист1!$B$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Лист1!$B$3:$B$37</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Лист1!$C$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Лист1!$C$3:$C$37</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Лист1!$O$28:$O$37</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Лист1!$P$28:$P$37</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Лист1!$P$28:$P$37</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Лист1!$O$28:$O$37</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Лист1!$P$28:$P$37</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Лист1!$O$28:$O$37</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Лист1!$P$28:$P$37</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Лист1!$O$28:$O$37</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Лист1!$P$28:$P$37</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Лист1!$B$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Лист1!$B$2:$B$57</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Лист1!$H$2:$H$57</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Лист1!$B$2:$B$57</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Лист1!$H$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Лист1!$H$2:$H$57</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Лист1!$B$2:$B$57</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Лист1!$H$1</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Лист1!$H$2:$H$57</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Лист1!$B$2:$B$57</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Лист1!$H$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Лист1!$H$2:$H$57</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Лист1!$H$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Лист1!$B$2:$B$57</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Лист1!$H$1</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Лист1!$H$2:$H$57</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Лист1!$B$1</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Лист1!$B$3:$B$37</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Лист1!$C$1</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Лист1!$C$3:$C$37</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Лист1!$B$2:$B$57</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Лист1!$H$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Лист1!$H$2:$H$57</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Лист1!$H$2:$H$57</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Лист1!$B$2:$B$57</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Лист1!$H$1</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Лист1!$H$2:$H$57</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Лист1!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Лист1!$B$2:$B$57</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Лист1!$H$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Лист1!$H$2:$H$57</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Лист1!$B$2:$B$57</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Лист1!$H$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Время</t>
   </si>
@@ -306,6 +313,18 @@
       <t>𝜎</t>
     </r>
   </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>𝛿</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
 </sst>
 </file>
 
@@ -535,18 +554,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -557,6 +564,21 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -583,9 +605,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -603,17 +622,1011 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$X$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$W$22:$W$57</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>4.8499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>4.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.88</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.91</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.92</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>4.93</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.95</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.96</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.97</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.01</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>5.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.03</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.0599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.07</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.09</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>5.1099999999999897</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.1199999999999903</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.1299999999999901</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>5.1399999999999899</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.1499999999999897</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.1599999999999904</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>5.1699999999999902</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.1799999999999899</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.1899999999999897</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>5.1999999999999904</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$X$22:$X$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>7.3864140198964506E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12010166274348749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18993310039662281</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29213834155947127</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.43703148489514859</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63587705844030207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.89984944188646443</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2385193926498728</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6579523132124538</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1586265944315364</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7335012445998896</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3666447592342963</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0328454086523564</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.6985312568383879</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.3241334253725361</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.867755446071647</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.2897204615498712</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.5573286016989867</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.6490380066905459</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.5573286016990036</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.2897204615499023</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.8677554460716905</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.3241334253725361</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.6985312568383879</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.0328454086524159</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.3666447592343549</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.7335012446005371</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.1586265944320639</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.6579523132129446</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.2385193926502762</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.89984944188678428</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.63587705844052644</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.43703148489532961</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.29213834155960117</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.18993310039671271</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.12010166274354296</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B733-F949-A716-1AD2D9F7E398}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="598358624"/>
+        <c:axId val="598352768"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="598358624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="598352768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="598352768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="598358624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$B$2:$B$57</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="56"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>4.8499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>4.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.88</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.91</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.92</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>4.93</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.95</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.96</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.97</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.01</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>5.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.03</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.0599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.07</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.09</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>5.1099999999999897</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.1199999999999903</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.1299999999999901</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>5.1399999999999899</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.1499999999999897</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.1599999999999904</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>5.1699999999999902</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.1799999999999899</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.1899999999999897</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>5.1999999999999904</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$H$2:$H$57</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="56"/>
+                <c:pt idx="0">
+                  <c:v>8.2055647777051549E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1693979458736671E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4255341283917782E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2835662921950619E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8725436461254941E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0811749465686231E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12178137908801209</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23069958156748444</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4134140713469468</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.7008034499875524</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1237759577717066</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7046521502019842</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4460443862289578</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.3202090211055064</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.263232771815372</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.1782760062821085</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.949820627379717</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.466884133823962</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.6490380066905459</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.466884133823994</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.9498206273797756</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.1782760062821858</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.263232771815372</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.3202090211055064</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4460443862290306</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.7046521502020433</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.1237759577722388</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.70080344998789501</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.41341407134719155</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.23069958156763473</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.12178137908809862</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.0811749465729176E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.8725436461278748E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.2835662921962032E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.4255341283969156E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.1693979458756707E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E71B-EC4D-AFD2-87105BE9F708}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1494474128"/>
+        <c:axId val="1494476400"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1494474128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1494476400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1494476400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1494474128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.24</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.26</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -624,7 +1637,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{62BEA4FC-3D34-3941-9DAF-50C06F2BBC35}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:f>_xlchart.v1.23</cx:f>
               <cx:v>Время</cx:v>
             </cx:txData>
           </cx:tx>
@@ -636,59 +1649,10 @@
         <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{A9161DC8-7A6B-AA4E-B708-B87958B43803}" formatIdx="1">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:f>_xlchart.v1.25</cx:f>
               <cx:v>Количество</cx:v>
             </cx:txData>
           </cx:tx>
-          <cx:dataId val="1"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="0"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-  </cx:chart>
-</cx:chartSpace>
-</file>
-
-<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="1">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="clusteredColumn" uniqueId="{19A2946A-9462-0A4D-9FE8-3D0A0A05F48E}" formatIdx="0">
-          <cx:dataPt idx="0"/>
-          <cx:dataPt idx="1"/>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r">
-              <cx:binCount val="4"/>
-            </cx:binning>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{C4882904-AB60-B548-AD67-540B510ED5F1}" formatIdx="1">
           <cx:dataId val="1"/>
           <cx:layoutPr>
             <cx:binning intervalClosed="r"/>
@@ -789,6 +1753,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
@@ -1298,33 +2302,27 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1332,14 +2330,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1347,7 +2345,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1355,28 +2353,24 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -1392,52 +2386,42 @@
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1446,22 +2430,22 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
@@ -1470,13 +2454,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1489,22 +2473,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -1535,58 +2516,57 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1600,12 +2580,92 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1613,109 +2673,24 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat">
-        <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
-        </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -1724,12 +2699,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1738,14 +2710,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1754,19 +2725,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1787,12 +2755,529 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -1801,6 +3286,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1809,13 +3300,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>685232</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>35825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>309919</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>191637</xdr:rowOff>
@@ -1855,7 +3346,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="7289232" y="645425"/>
-              <a:ext cx="4577687" cy="2797412"/>
+              <a:ext cx="4666587" cy="2797412"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1887,13 +3378,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>330200</xdr:rowOff>
@@ -1958,13 +3449,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -2030,79 +3521,125 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>731655</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>128798</xdr:rowOff>
+      <xdr:colOff>179717</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>325930</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>134866</xdr:rowOff>
+      <xdr:colOff>566964</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>154189</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="9" name="Диаграмма 8">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9A4F43D-98CA-9532-07AC-C3DF9DECEC4B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="13948646" y="5073931"/>
-              <a:ext cx="4618080" cy="4119519"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="ru-RU" sz="1100"/>
-                <a:t>Эта диаграмма недоступна в вашей версии Excel.
-Изменение этой фигуры или сохранение книги в другом формате приведет к остаточному повреждению диаграммы.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Диаграмма 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3167D712-4306-6CD8-E0D4-822F014D05CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>340179</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>11339</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>200026</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>13154</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Рисунок 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C94A5DD3-2D14-603A-8181-D3812E3E52EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:duotone>
+            <a:prstClr val="black"/>
+            <a:srgbClr val="FF0000">
+              <a:tint val="45000"/>
+              <a:satMod val="400000"/>
+            </a:srgbClr>
+          </a:duotone>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7790090" y="827768"/>
+          <a:ext cx="4089400" cy="2451100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>767080</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>690880</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>406400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Диаграмма 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0112440-0836-AD5A-54CD-0FB299050643}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2405,20 +3942,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0F376C-AF39-7E44-8D33-F1A63A254D50}">
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:AE57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I19" zoomScale="113" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28:P37"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2432,7 +3969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2458,16 +3995,20 @@
         <f>F2*F2</f>
         <v>3.0834071206127314E-2</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
+        <f>(1/$K$32/SQRTPI(2))*EXP(-((B2-$K$34)^2)/($K$32^2))</f>
+        <v>8.2055647777051549E-4</v>
+      </c>
+      <c r="I2" s="1">
         <f>SQRT(1/108/108*SUM(G:G))</f>
         <v>5.7713699179505369E-3</v>
       </c>
-      <c r="I2" s="1">
-        <f>1/H2/SQRT(PI()*2)</f>
+      <c r="J2" s="1">
+        <f>1/I2/SQRT(PI()*2)</f>
         <v>69.12436493814289</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2486,11 +4027,15 @@
         <v>-0.16559633027522835</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G37" si="2">F3*F3</f>
+        <f>F3*F3</f>
         <v>2.7422144600622509E-2</v>
       </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H37" si="2">(1/$K$32/SQRTPI(2))*EXP(-((B3-$K$34)^2)/($K$32^2))</f>
+        <v>2.1693979458736671E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2509,11 +4054,15 @@
         <v>-0.15559633027522857</v>
       </c>
       <c r="G4" s="2">
+        <f>F4*F4</f>
+        <v>2.4210217995118011E-2</v>
+      </c>
+      <c r="H4" s="2">
         <f t="shared" si="2"/>
-        <v>2.4210217995118011E-2</v>
+        <v>5.4255341283917782E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2532,15 +4081,19 @@
         <v>-0.14559633027522878</v>
       </c>
       <c r="G5" s="2">
+        <f>F5*F5</f>
+        <v>2.1198291389613502E-2</v>
+      </c>
+      <c r="H5" s="2">
         <f t="shared" si="2"/>
-        <v>2.1198291389613502E-2</v>
-      </c>
-      <c r="H5">
+        <v>1.2835662921950619E-2</v>
+      </c>
+      <c r="I5">
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2559,11 +4112,15 @@
         <v>-0.13559633027522899</v>
       </c>
       <c r="G6" s="2">
+        <f>F6*F6</f>
+        <v>1.8386364784108981E-2</v>
+      </c>
+      <c r="H6" s="2">
         <f t="shared" si="2"/>
-        <v>1.8386364784108981E-2</v>
+        <v>2.8725436461254941E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2582,11 +4139,15 @@
         <v>-0.12559633027522832</v>
       </c>
       <c r="G7" s="2">
+        <f>F7*F7</f>
+        <v>1.5774438178604234E-2</v>
+      </c>
+      <c r="H7" s="2">
         <f t="shared" si="2"/>
-        <v>1.5774438178604234E-2</v>
+        <v>6.0811749465686231E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2605,11 +4166,15 @@
         <v>-0.11559633027522853</v>
       </c>
       <c r="G8" s="2">
+        <f>F8*F8</f>
+        <v>1.3362511573099716E-2</v>
+      </c>
+      <c r="H8" s="2">
         <f t="shared" si="2"/>
-        <v>1.3362511573099716E-2</v>
+        <v>0.12178137908801209</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2628,15 +4193,19 @@
         <v>-0.10559633027522874</v>
       </c>
       <c r="G9" s="2">
+        <f>F9*F9</f>
+        <v>1.1150584967595191E-2</v>
+      </c>
+      <c r="H9" s="2">
         <f t="shared" si="2"/>
-        <v>1.1150584967595191E-2</v>
-      </c>
-      <c r="H9">
+        <v>0.23069958156748444</v>
+      </c>
+      <c r="I9">
         <f>6.65*0.01</f>
         <v>6.6500000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2655,11 +4224,15 @@
         <v>-9.5596330275228958E-2</v>
       </c>
       <c r="G10" s="2">
+        <f>F10*F10</f>
+        <v>9.138658362090657E-3</v>
+      </c>
+      <c r="H10" s="2">
         <f t="shared" si="2"/>
-        <v>9.138658362090657E-3</v>
+        <v>0.4134140713469468</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2678,11 +4251,15 @@
         <v>-8.5596330275228283E-2</v>
       </c>
       <c r="G11" s="2">
+        <f>F11*F11</f>
+        <v>7.3267317565859618E-3</v>
+      </c>
+      <c r="H11" s="2">
         <f t="shared" si="2"/>
-        <v>7.3267317565859618E-3</v>
+        <v>0.7008034499875524</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2701,11 +4278,15 @@
         <v>-7.5596330275228496E-2</v>
       </c>
       <c r="G12" s="2">
+        <f>F12*F12</f>
+        <v>5.7148051510814285E-3</v>
+      </c>
+      <c r="H12" s="2">
         <f t="shared" si="2"/>
-        <v>5.7148051510814285E-3</v>
+        <v>1.1237759577717066</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2724,11 +4305,15 @@
         <v>-6.5596330275228709E-2</v>
       </c>
       <c r="G13" s="2">
+        <f>F13*F13</f>
+        <v>4.3028785455768862E-3</v>
+      </c>
+      <c r="H13" s="2">
         <f t="shared" si="2"/>
-        <v>4.3028785455768862E-3</v>
+        <v>1.7046521502019842</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2747,11 +4332,15 @@
         <v>-5.5596330275228922E-2</v>
       </c>
       <c r="G14" s="2">
+        <f>F14*F14</f>
+        <v>3.0909519400723361E-3</v>
+      </c>
+      <c r="H14" s="2">
         <f t="shared" si="2"/>
-        <v>3.0909519400723361E-3</v>
+        <v>2.4460443862289578</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2770,11 +4359,15 @@
         <v>-4.5596330275228247E-2</v>
       </c>
       <c r="G15" s="2">
+        <f>F15*F15</f>
+        <v>2.079025334567696E-3</v>
+      </c>
+      <c r="H15" s="2">
         <f t="shared" si="2"/>
-        <v>2.079025334567696E-3</v>
+        <v>3.3202090211055064</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2793,11 +4386,15 @@
         <v>-3.559633027522846E-2</v>
       </c>
       <c r="G16" s="2">
+        <f>F16*F16</f>
+        <v>1.2670987290631464E-3</v>
+      </c>
+      <c r="H16" s="2">
         <f t="shared" si="2"/>
-        <v>1.2670987290631464E-3</v>
+        <v>4.263232771815372</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2816,11 +4413,15 @@
         <v>-2.5596330275228674E-2</v>
       </c>
       <c r="G17" s="2">
+        <f>F17*F17</f>
+        <v>6.5517212355858804E-4</v>
+      </c>
+      <c r="H17" s="2">
         <f t="shared" si="2"/>
-        <v>6.5517212355858804E-4</v>
+        <v>5.1782760062821085</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2839,14 +4440,18 @@
         <v>-1.5596330275228887E-2</v>
       </c>
       <c r="G18" s="2">
+        <f>F18*F18</f>
+        <v>2.4324551805402116E-4</v>
+      </c>
+      <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>2.4324551805402116E-4</v>
-      </c>
-      <c r="I18" s="7" t="s">
+        <v>5.949820627379717</v>
+      </c>
+      <c r="J18" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2865,12 +4470,16 @@
         <v>-5.5963302752291E-3</v>
       </c>
       <c r="G19" s="2">
+        <f>F19*F19</f>
+        <v>3.1318912549445813E-5</v>
+      </c>
+      <c r="H19" s="2">
         <f t="shared" si="2"/>
-        <v>3.1318912549445813E-5</v>
-      </c>
-      <c r="O19" s="13"/>
+        <v>6.466884133823962</v>
+      </c>
+      <c r="P19" s="9"/>
     </row>
-    <row r="20" spans="1:20" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2889,29 +4498,33 @@
         <v>4.403669724771575E-3</v>
       </c>
       <c r="G20" s="2">
+        <f>F20*F20</f>
+        <v>1.9392307044869761E-5</v>
+      </c>
+      <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>1.9392307044869761E-5</v>
-      </c>
-      <c r="I20" s="3" t="s">
+        <v>6.6490380066905459</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="6" t="s">
+      <c r="M20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="N20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O20" s="14" t="s">
+      <c r="P20" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2930,41 +4543,57 @@
         <v>1.4403669724771362E-2</v>
       </c>
       <c r="G21" s="2">
+        <f>F21*F21</f>
+        <v>2.0746570154029511E-4</v>
+      </c>
+      <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>2.0746570154029511E-4</v>
-      </c>
-      <c r="I21" s="8">
+        <v>6.466884133823994</v>
+      </c>
+      <c r="J21" s="8">
         <v>4.8600000000000003</v>
       </c>
-      <c r="J21" s="11">
+      <c r="K21" s="14">
         <v>13</v>
       </c>
-      <c r="K21" s="9">
-        <f>J21/109/0.06</f>
+      <c r="L21" s="16">
+        <f>K21/109/0.06</f>
         <v>1.9877675840978595</v>
       </c>
-      <c r="L21" s="9">
+      <c r="M21" s="16">
         <f>SUM(D3:D9)/SUM(C3:C9)</f>
         <v>4.8999999999999995</v>
       </c>
-      <c r="M21" s="9">
-        <f>1/$J$32/SQRTPI(2)*EXP(-(L21-$J$34)*(L21-$J$34)/2/$J$32/$J$32)</f>
+      <c r="N21" s="16">
+        <f>1/$K$32/SQRTPI(2)*EXP(-(M21-$K$34)*(M21-$K$34)/2/$K$32/$K$32)</f>
         <v>0.63587705844028142</v>
       </c>
-      <c r="O21" s="17"/>
-      <c r="P21" s="19" t="s">
+      <c r="P21" s="18"/>
+      <c r="Q21" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="21" t="s">
+      <c r="R21" s="21"/>
+      <c r="S21" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="S21" s="23"/>
-      <c r="T21" s="21" t="s">
+      <c r="T21" s="24"/>
+      <c r="U21" s="22" t="s">
         <v>14</v>
       </c>
+      <c r="W21" t="s">
+        <v>23</v>
+      </c>
+      <c r="X21" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>5.03</v>
+      </c>
     </row>
-    <row r="22" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2983,28 +4612,45 @@
         <v>2.4403669724771149E-2</v>
       </c>
       <c r="G22" s="2">
+        <f>F22*F22</f>
+        <v>5.955390960357119E-4</v>
+      </c>
+      <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>5.955390960357119E-4</v>
-      </c>
-      <c r="I22" s="8">
+        <v>5.9498206273797756</v>
+      </c>
+      <c r="J22" s="8">
         <v>4.92</v>
       </c>
-      <c r="J22" s="12"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="15" t="s">
+      <c r="K22" s="15"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q22" s="15" t="s">
+      <c r="R22" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R22" s="22"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="22"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="23"/>
+      <c r="W22">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="X22">
+        <f>1/$AE$22/SQRTPI(2)*EXP(-((W22-$AE$21)^2)/(2*$AE$22^2))</f>
+        <v>7.3864140198964506E-2</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>0.06</v>
+      </c>
     </row>
-    <row r="23" spans="1:20" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3023,51 +4669,62 @@
         <v>3.4403669724770936E-2</v>
       </c>
       <c r="G23" s="2">
+        <f>F23*F23</f>
+        <v>1.1836124905311202E-3</v>
+      </c>
+      <c r="H23" s="2">
         <f t="shared" si="2"/>
-        <v>1.1836124905311202E-3</v>
-      </c>
-      <c r="I23" s="8">
+        <v>5.1782760062821858</v>
+      </c>
+      <c r="J23" s="8">
         <v>4.93</v>
       </c>
-      <c r="J23" s="11">
+      <c r="K23" s="14">
         <v>25</v>
       </c>
-      <c r="K23" s="9">
-        <f>J23/109/0.06</f>
+      <c r="L23" s="16">
+        <f>K23/109/0.06</f>
         <v>3.8226299694189607</v>
       </c>
-      <c r="L23" s="9">
+      <c r="M23" s="16">
         <f>SUM(D10:D16)/SUM(C10:C16)</f>
         <v>4.9676</v>
       </c>
-      <c r="M23" s="9">
-        <f t="shared" ref="M23" si="3">1/$J$32/SQRTPI(2)*EXP(-(L23-$J$34)*(L23-$J$34)/2/$J$32/$J$32)</f>
+      <c r="N23" s="16">
+        <f t="shared" ref="N23" si="3">1/$K$32/SQRTPI(2)*EXP(-(M23-$K$34)*(M23-$K$34)/2/$K$32/$K$32)</f>
         <v>3.8716167457227546</v>
       </c>
-      <c r="O23" s="16" t="s">
+      <c r="P23" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="P23" s="15">
-        <f>$J$34-$J$32</f>
+      <c r="Q23" s="11">
+        <f>$K$34-$K$32</f>
         <v>4.9700000000000006</v>
       </c>
-      <c r="Q23" s="15">
-        <f>$J$34+$J$32</f>
+      <c r="R23" s="11">
+        <f>$K$34+$K$32</f>
         <v>5.09</v>
       </c>
-      <c r="R23" s="15">
+      <c r="S23" s="11">
         <f>SUM(C14:C26)</f>
         <v>64</v>
       </c>
-      <c r="S23" s="25">
-        <f>R23/109</f>
+      <c r="T23" s="13">
+        <f>S23/109</f>
         <v>0.58715596330275233</v>
       </c>
-      <c r="T23" s="15">
+      <c r="U23" s="11">
         <v>0.68300000000000005</v>
       </c>
+      <c r="W23" s="1">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="X23">
+        <f t="shared" ref="X23:X57" si="4">1/$AE$22/SQRTPI(2)*EXP(-((W23-$AE$21)^2)/(2*$AE$22^2))</f>
+        <v>0.12010166274348749</v>
+      </c>
     </row>
-    <row r="24" spans="1:20" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3086,40 +4743,51 @@
         <v>4.4403669724771611E-2</v>
       </c>
       <c r="G24" s="2">
+        <f>F24*F24</f>
+        <v>1.9716858850265988E-3</v>
+      </c>
+      <c r="H24" s="2">
         <f t="shared" si="2"/>
-        <v>1.9716858850265988E-3</v>
-      </c>
-      <c r="I24" s="8">
+        <v>4.263232771815372</v>
+      </c>
+      <c r="J24" s="8">
         <v>4.99</v>
       </c>
-      <c r="J24" s="12"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="O24" s="16" t="s">
+      <c r="K24" s="15"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="P24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P24" s="15">
-        <f>$J$34-2*$J$32</f>
+      <c r="Q24" s="11">
+        <f>$K$34-2*$K$32</f>
         <v>4.91</v>
       </c>
-      <c r="Q24" s="15">
-        <f>$J$34+2*$J$32</f>
+      <c r="R24" s="11">
+        <f>$K$34+2*$K$32</f>
         <v>5.15</v>
       </c>
-      <c r="R24" s="15">
+      <c r="S24" s="11">
         <f>SUM(C8:C32)</f>
         <v>94</v>
       </c>
-      <c r="S24" s="25">
-        <f t="shared" ref="S24:S25" si="4">R24/109</f>
+      <c r="T24" s="13">
+        <f t="shared" ref="T24:T25" si="5">S24/109</f>
         <v>0.86238532110091748</v>
       </c>
-      <c r="T24" s="15">
+      <c r="U24" s="11">
         <v>0.95399999999999996</v>
       </c>
+      <c r="W24">
+        <v>4.87</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="4"/>
+        <v>0.18993310039662281</v>
+      </c>
     </row>
-    <row r="25" spans="1:20" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3138,51 +4806,62 @@
         <v>5.4403669724771397E-2</v>
       </c>
       <c r="G25" s="2">
+        <f>F25*F25</f>
+        <v>2.9597592795220081E-3</v>
+      </c>
+      <c r="H25" s="2">
         <f t="shared" si="2"/>
-        <v>2.9597592795220081E-3</v>
-      </c>
-      <c r="I25" s="8">
+        <v>3.3202090211055064</v>
+      </c>
+      <c r="J25" s="8">
         <v>5</v>
       </c>
-      <c r="J25" s="11">
+      <c r="K25" s="14">
         <v>40</v>
       </c>
-      <c r="K25" s="9">
-        <f t="shared" ref="K25" si="5">J25/109/0.06</f>
+      <c r="L25" s="16">
+        <f t="shared" ref="L25" si="6">K25/109/0.06</f>
         <v>6.1162079510703373</v>
       </c>
-      <c r="L25" s="9">
+      <c r="M25" s="16">
         <f>SUM(D17:D23)/SUM(C17:C23)</f>
         <v>5.0272500000000004</v>
       </c>
-      <c r="M25" s="9">
-        <f t="shared" ref="M25" si="6">1/$J$32/SQRTPI(2)*EXP(-(L25-$J$34)*(L25-$J$34)/2/$J$32/$J$32)</f>
+      <c r="N25" s="16">
+        <f t="shared" ref="N25" si="7">1/$K$32/SQRTPI(2)*EXP(-(M25-$K$34)*(M25-$K$34)/2/$K$32/$K$32)</f>
         <v>6.642057874512715</v>
       </c>
-      <c r="O25" s="16" t="s">
+      <c r="P25" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="P25" s="15">
-        <f>$J$34-3*$J$32</f>
+      <c r="Q25" s="11">
+        <f>$K$34-3*$K$32</f>
         <v>4.8500000000000005</v>
       </c>
-      <c r="Q25" s="15">
-        <f>$J$34+3*$J$32</f>
+      <c r="R25" s="11">
+        <f>$K$34+3*$K$32</f>
         <v>5.21</v>
       </c>
-      <c r="R25" s="15">
+      <c r="S25" s="11">
         <f>SUM(C2:C37)</f>
         <v>109</v>
       </c>
-      <c r="S25" s="25">
+      <c r="T25" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U25" s="11">
+        <v>0.997</v>
+      </c>
+      <c r="W25" s="1">
+        <v>4.88</v>
+      </c>
+      <c r="X25">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="T25" s="15">
-        <v>0.997</v>
+        <v>0.29213834155947127</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3201,19 +4880,30 @@
         <v>6.4403669724771184E-2</v>
       </c>
       <c r="G26" s="2">
+        <f>F26*F26</f>
+        <v>4.1478326740174085E-3</v>
+      </c>
+      <c r="H26" s="2">
         <f t="shared" si="2"/>
-        <v>4.1478326740174085E-3</v>
-      </c>
-      <c r="I26" s="8">
+        <v>2.4460443862290306</v>
+      </c>
+      <c r="J26" s="8">
         <v>5.0599999999999996</v>
       </c>
-      <c r="J26" s="12"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="O26" s="13"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="P26" s="9"/>
+      <c r="W26" s="1">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="4"/>
+        <v>0.43703148489514859</v>
+      </c>
     </row>
-    <row r="27" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3232,29 +4922,40 @@
         <v>7.4403669724770971E-2</v>
       </c>
       <c r="G27" s="2">
+        <f>F27*F27</f>
+        <v>5.5359060685128006E-3</v>
+      </c>
+      <c r="H27" s="2">
         <f t="shared" si="2"/>
-        <v>5.5359060685128006E-3</v>
-      </c>
-      <c r="I27" s="8">
+        <v>1.7046521502020433</v>
+      </c>
+      <c r="J27" s="8">
         <v>5.07</v>
       </c>
-      <c r="J27" s="11">
+      <c r="K27" s="14">
         <v>19</v>
       </c>
-      <c r="K27" s="9">
-        <f t="shared" ref="K27" si="7">J27/109/0.06</f>
+      <c r="L27" s="16">
+        <f t="shared" ref="L27" si="8">K27/109/0.06</f>
         <v>2.90519877675841</v>
       </c>
-      <c r="L27" s="9">
+      <c r="M27" s="16">
         <f>SUM(D24:D30)/SUM(C24:C30)</f>
         <v>5.0984210526315756</v>
       </c>
-      <c r="M27" s="9">
-        <f t="shared" ref="M27" si="8">1/$J$32/SQRTPI(2)*EXP(-(L27-$J$34)*(L27-$J$34)/2/$J$32/$J$32)</f>
+      <c r="N27" s="16">
+        <f t="shared" ref="N27" si="9">1/$K$32/SQRTPI(2)*EXP(-(M27-$K$34)*(M27-$K$34)/2/$K$32/$K$32)</f>
         <v>3.4704078462624532</v>
       </c>
+      <c r="W27">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="4"/>
+        <v>0.63587705844030207</v>
+      </c>
     </row>
-    <row r="28" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3273,24 +4974,35 @@
         <v>8.4403669724760988E-2</v>
       </c>
       <c r="G28" s="2">
+        <f>F28*F28</f>
+        <v>7.1239794630065349E-3</v>
+      </c>
+      <c r="H28" s="2">
         <f t="shared" si="2"/>
-        <v>7.1239794630065349E-3</v>
-      </c>
-      <c r="I28" s="8">
+        <v>1.1237759577722388</v>
+      </c>
+      <c r="J28" s="8">
         <v>5.13</v>
       </c>
-      <c r="J28" s="12"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="O28" s="9">
+      <c r="K28" s="15"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="P28" s="16">
         <v>4.8999999999999995</v>
       </c>
-      <c r="P28" s="9">
+      <c r="Q28" s="16">
         <v>1.9877675840978595</v>
       </c>
+      <c r="W28" s="1">
+        <v>4.91</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="4"/>
+        <v>0.89984944188646443</v>
+      </c>
     </row>
-    <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3309,31 +5021,42 @@
         <v>9.4403669724761663E-2</v>
       </c>
       <c r="G29" s="2">
+        <f>F29*F29</f>
+        <v>8.9120528575018822E-3</v>
+      </c>
+      <c r="H29" s="2">
         <f t="shared" si="2"/>
-        <v>8.9120528575018822E-3</v>
-      </c>
-      <c r="I29" s="8">
+        <v>0.70080344998789501</v>
+      </c>
+      <c r="J29" s="8">
         <v>5.14</v>
       </c>
-      <c r="J29" s="11">
+      <c r="K29" s="14">
         <v>12</v>
       </c>
-      <c r="K29" s="9">
-        <f t="shared" ref="K29" si="9">J29/109/0.06</f>
+      <c r="L29" s="16">
+        <f t="shared" ref="L29" si="10">K29/109/0.06</f>
         <v>1.834862385321101</v>
       </c>
-      <c r="L29" s="9">
+      <c r="M29" s="16">
         <f>SUM(D31:D37)/SUM(C31:C37)</f>
         <v>5.1616666666666564</v>
       </c>
-      <c r="M29" s="9">
-        <f>1/$J$32/SQRTPI(2)*EXP(-(L29-$J$34)*(L29-$J$34)/2/$J$32/$J$32)</f>
+      <c r="N29" s="16">
+        <f>1/$K$32/SQRTPI(2)*EXP(-(M29-$K$34)*(M29-$K$34)/2/$K$32/$K$32)</f>
         <v>0.59850462502436352</v>
       </c>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="W29" s="1">
+        <v>4.92</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="4"/>
+        <v>1.2385193926498728</v>
+      </c>
     </row>
-    <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3352,24 +5075,35 @@
         <v>0.10440366972476145</v>
       </c>
       <c r="G30" s="2">
+        <f>F30*F30</f>
+        <v>1.090012625199707E-2</v>
+      </c>
+      <c r="H30" s="2">
         <f t="shared" si="2"/>
-        <v>1.090012625199707E-2</v>
-      </c>
-      <c r="I30" s="8">
+        <v>0.41341407134719155</v>
+      </c>
+      <c r="J30" s="8">
         <v>5.2</v>
       </c>
-      <c r="J30" s="12"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="O30" s="9">
+      <c r="K30" s="15"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="P30" s="16">
         <v>4.9676</v>
       </c>
-      <c r="P30" s="9">
+      <c r="Q30" s="16">
         <v>3.8226299694189607</v>
       </c>
+      <c r="W30">
+        <v>4.93</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="4"/>
+        <v>1.6579523132124538</v>
+      </c>
     </row>
-    <row r="31" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3388,13 +5122,24 @@
         <v>0.11440366972476124</v>
       </c>
       <c r="G31" s="2">
+        <f>F31*F31</f>
+        <v>1.308819964649225E-2</v>
+      </c>
+      <c r="H31" s="2">
         <f t="shared" si="2"/>
-        <v>1.308819964649225E-2</v>
-      </c>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
+        <v>0.23069958156763473</v>
+      </c>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="W31" s="1">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="4"/>
+        <v>2.1586265944315364</v>
+      </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3413,23 +5158,34 @@
         <v>0.12440366972476102</v>
       </c>
       <c r="G32" s="2">
+        <f>F32*F32</f>
+        <v>1.5476273040987422E-2</v>
+      </c>
+      <c r="H32" s="2">
         <f t="shared" si="2"/>
-        <v>1.5476273040987422E-2</v>
-      </c>
-      <c r="I32" t="s">
+        <v>0.12178137908809862</v>
+      </c>
+      <c r="J32" t="s">
         <v>10</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>0.06</v>
       </c>
-      <c r="O32" s="9">
+      <c r="P32" s="16">
         <v>5.0272500000000004</v>
       </c>
-      <c r="P32" s="9">
+      <c r="Q32" s="16">
         <v>6.1162079510703373</v>
       </c>
+      <c r="W32" s="1">
+        <v>4.95</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="4"/>
+        <v>2.7335012445998896</v>
+      </c>
     </row>
-    <row r="33" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3448,19 +5204,30 @@
         <v>0.1344036697247617</v>
       </c>
       <c r="G33" s="2">
+        <f>F33*F33</f>
+        <v>1.8064346435482825E-2</v>
+      </c>
+      <c r="H33" s="2">
         <f t="shared" si="2"/>
-        <v>1.8064346435482825E-2</v>
-      </c>
-      <c r="I33" t="s">
+        <v>6.0811749465729176E-2</v>
+      </c>
+      <c r="J33" t="s">
         <v>11</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>3.14</v>
       </c>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="W33">
+        <v>4.96</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="4"/>
+        <v>3.3666447592342963</v>
+      </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3479,23 +5246,34 @@
         <v>0.14440366972476149</v>
       </c>
       <c r="G34" s="2">
+        <f>F34*F34</f>
+        <v>2.0852419829977997E-2</v>
+      </c>
+      <c r="H34" s="2">
         <f t="shared" si="2"/>
-        <v>2.0852419829977997E-2</v>
-      </c>
-      <c r="I34" t="s">
+        <v>2.8725436461278748E-2</v>
+      </c>
+      <c r="J34" t="s">
         <v>12</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>5.03</v>
       </c>
-      <c r="O34" s="9">
+      <c r="P34" s="16">
         <v>5.0984210526315756</v>
       </c>
-      <c r="P34" s="9">
+      <c r="Q34" s="16">
         <v>2.90519877675841</v>
       </c>
+      <c r="W34" s="1">
+        <v>4.97</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="4"/>
+        <v>4.0328454086523564</v>
+      </c>
     </row>
-    <row r="35" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3514,13 +5292,24 @@
         <v>0.15440366972476127</v>
       </c>
       <c r="G35" s="2">
+        <f>F35*F35</f>
+        <v>2.384049322447316E-2</v>
+      </c>
+      <c r="H35" s="2">
         <f t="shared" si="2"/>
-        <v>2.384049322447316E-2</v>
-      </c>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
+        <v>1.2835662921962032E-2</v>
+      </c>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="W35" s="1">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="4"/>
+        <v>4.6985312568383879</v>
+      </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3539,17 +5328,28 @@
         <v>0.16440366972476106</v>
       </c>
       <c r="G36" s="2">
+        <f>F36*F36</f>
+        <v>2.7028566618968314E-2</v>
+      </c>
+      <c r="H36" s="2">
         <f t="shared" si="2"/>
-        <v>2.7028566618968314E-2</v>
-      </c>
-      <c r="O36" s="9">
+        <v>5.4255341283969156E-3</v>
+      </c>
+      <c r="P36" s="16">
         <v>5.1616666666666564</v>
       </c>
-      <c r="P36" s="9">
+      <c r="Q36" s="16">
         <v>1.834862385321101</v>
       </c>
+      <c r="W36">
+        <v>4.99</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="4"/>
+        <v>5.3241334253725361</v>
+      </c>
     </row>
-    <row r="37" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3568,49 +5368,240 @@
         <v>0.17440366972476173</v>
       </c>
       <c r="G37" s="2">
+        <f>F37*F37</f>
+        <v>3.0416640013463773E-2</v>
+      </c>
+      <c r="H37" s="2">
         <f t="shared" si="2"/>
-        <v>3.0416640013463773E-2</v>
-      </c>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
+        <v>2.1693979458756707E-3</v>
+      </c>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="W37" s="1">
+        <v>5</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="4"/>
+        <v>5.867755446071647</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W38" s="1">
+        <v>5.01</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="4"/>
+        <v>6.2897204615498712</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W39">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="4"/>
+        <v>6.5573286016989867</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W40" s="1">
+        <v>5.03</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="4"/>
+        <v>6.6490380066905459</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W41" s="1">
+        <v>5.04</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="4"/>
+        <v>6.5573286016990036</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W42">
+        <v>5.05</v>
+      </c>
+      <c r="X42">
+        <f t="shared" si="4"/>
+        <v>6.2897204615499023</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W43" s="1">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="X43">
+        <f t="shared" si="4"/>
+        <v>5.8677554460716905</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W44" s="1">
+        <v>5.07</v>
+      </c>
+      <c r="X44">
+        <f t="shared" si="4"/>
+        <v>5.3241334253725361</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W45">
+        <v>5.08</v>
+      </c>
+      <c r="X45">
+        <f t="shared" si="4"/>
+        <v>4.6985312568383879</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W46" s="1">
+        <v>5.09</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="4"/>
+        <v>4.0328454086524159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W47" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="4"/>
+        <v>3.3666447592343549</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="W48">
+        <v>5.1099999999999897</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="4"/>
+        <v>2.7335012446005371</v>
+      </c>
+    </row>
+    <row r="49" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W49" s="1">
+        <v>5.1199999999999903</v>
+      </c>
+      <c r="X49">
+        <f t="shared" si="4"/>
+        <v>2.1586265944320639</v>
+      </c>
+    </row>
+    <row r="50" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W50" s="1">
+        <v>5.1299999999999901</v>
+      </c>
+      <c r="X50">
+        <f t="shared" si="4"/>
+        <v>1.6579523132129446</v>
+      </c>
+    </row>
+    <row r="51" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W51">
+        <v>5.1399999999999899</v>
+      </c>
+      <c r="X51">
+        <f t="shared" si="4"/>
+        <v>1.2385193926502762</v>
+      </c>
+    </row>
+    <row r="52" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W52" s="1">
+        <v>5.1499999999999897</v>
+      </c>
+      <c r="X52">
+        <f t="shared" si="4"/>
+        <v>0.89984944188678428</v>
+      </c>
+    </row>
+    <row r="53" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W53" s="1">
+        <v>5.1599999999999904</v>
+      </c>
+      <c r="X53">
+        <f t="shared" si="4"/>
+        <v>0.63587705844052644</v>
+      </c>
+    </row>
+    <row r="54" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W54">
+        <v>5.1699999999999902</v>
+      </c>
+      <c r="X54">
+        <f t="shared" si="4"/>
+        <v>0.43703148489532961</v>
+      </c>
+    </row>
+    <row r="55" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W55" s="1">
+        <v>5.1799999999999899</v>
+      </c>
+      <c r="X55">
+        <f t="shared" si="4"/>
+        <v>0.29213834155960117</v>
+      </c>
+    </row>
+    <row r="56" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W56" s="1">
+        <v>5.1899999999999897</v>
+      </c>
+      <c r="X56">
+        <f t="shared" si="4"/>
+        <v>0.18993310039671271</v>
+      </c>
+    </row>
+    <row r="57" spans="23:24" x14ac:dyDescent="0.2">
+      <c r="W57">
+        <v>5.1999999999999904</v>
+      </c>
+      <c r="X57">
+        <f t="shared" si="4"/>
+        <v>0.12010166274354296</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="Q30:Q31"/>
+    <mergeCell ref="Q32:Q33"/>
+    <mergeCell ref="Q34:Q35"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="P28:P29"/>
     <mergeCell ref="P30:P31"/>
     <mergeCell ref="P32:P33"/>
     <mergeCell ref="P34:P35"/>
     <mergeCell ref="P36:P37"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="O32:O33"/>
-    <mergeCell ref="O34:O35"/>
-    <mergeCell ref="O36:O37"/>
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:R22"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="Q21:R21"/>
     <mergeCell ref="S21:S22"/>
     <mergeCell ref="T21:T22"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="U21:U22"/>
     <mergeCell ref="K29:K30"/>
     <mergeCell ref="L29:L30"/>
     <mergeCell ref="M29:M30"/>
-    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="N29:N30"/>
     <mergeCell ref="K25:K26"/>
     <mergeCell ref="L25:L26"/>
     <mergeCell ref="M25:M26"/>
-    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="N25:N26"/>
     <mergeCell ref="K27:K28"/>
     <mergeCell ref="L27:L28"/>
     <mergeCell ref="M27:M28"/>
-    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="N27:N28"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="M21:M22"/>
-    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="N21:N22"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="M23:M24"/>
+    <mergeCell ref="N23:N24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>